<commit_message>
Made changes according to feedback for A/B testing final project. Finalized documentation uploaded.
</commit_message>
<xml_diff>
--- a/8 DesignAnABTest/Final Project Baseline Values.xlsx
+++ b/8 DesignAnABTest/Final Project Baseline Values.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>Unique cookies to view page per day:</t>
   </si>
@@ -66,9 +66,6 @@
     <t>Standard error</t>
   </si>
   <si>
-    <t>How many page views will you need?</t>
-  </si>
-  <si>
     <t>Alpha</t>
   </si>
   <si>
@@ -78,14 +75,41 @@
     <t>Calculator</t>
   </si>
   <si>
-    <t>Min sample size</t>
+    <t>Min sample size based on UOD</t>
+  </si>
+  <si>
+    <t>Metrics</t>
+  </si>
+  <si>
+    <t>Min sample size pageviews</t>
+  </si>
+  <si>
+    <t>Min sample size per group</t>
+  </si>
+  <si>
+    <t>&lt;- too many pageviews</t>
+  </si>
+  <si>
+    <t>How many page views do you need?</t>
+  </si>
+  <si>
+    <t>Fraction of traffic?</t>
+  </si>
+  <si>
+    <t>Number of days</t>
+  </si>
+  <si>
+    <t>Fraction of traffic</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.00000000"/>
+  </numFmts>
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -94,6 +118,7 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -105,6 +130,12 @@
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -129,12 +160,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -415,19 +448,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="D1" sqref="A1:D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="40.109375" customWidth="1"/>
     <col min="4" max="4" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="35.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="B1" s="3" t="s">
         <v>10</v>
       </c>
@@ -438,10 +478,16 @@
         <v>14</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -453,11 +499,9 @@
         <v>5000</v>
       </c>
       <c r="D2" s="2"/>
-      <c r="F2" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E2" s="2"/>
+    </row>
+    <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -468,11 +512,8 @@
         <f>C2*B5</f>
         <v>400</v>
       </c>
-      <c r="F3" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -484,7 +525,7 @@
         <v>82.5</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -493,7 +534,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -501,20 +542,23 @@
         <f t="shared" si="0"/>
         <v>0.20624999999999999</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="6">
         <f>SQRT(B6*(1-B6)/C3)</f>
         <v>2.0230604137049392E-2</v>
       </c>
       <c r="E6">
-        <f>25835*2</f>
+        <v>25835</v>
+      </c>
+      <c r="F6">
+        <f>E6*2</f>
         <v>51670</v>
       </c>
-      <c r="F6">
-        <f>E6/B5</f>
+      <c r="G6">
+        <f>F6/B5</f>
         <v>645875</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -526,15 +570,21 @@
         <v>5.4949012178509081E-2</v>
       </c>
       <c r="E7">
-        <f>39087*2</f>
+        <v>39087</v>
+      </c>
+      <c r="F7">
+        <f>E7*2</f>
         <v>78174</v>
       </c>
-      <c r="F7" s="4">
-        <f>E7/(B4/B2)</f>
+      <c r="G7" s="4">
+        <f>F7/(B4/B2)</f>
         <v>4737818.1818181816</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H7" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -542,51 +592,95 @@
         <f>B6*B7</f>
         <v>0.10931249999999999</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="6">
         <f>SQRT(B8*(1-B8)/C3)</f>
         <v>1.5601544582488459E-2</v>
       </c>
       <c r="E8">
+        <v>27413</v>
+      </c>
+      <c r="F8">
+        <f>E8*2</f>
         <v>54826</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="G8" s="3">
+        <f>F8/B5</f>
+        <v>685325</v>
+      </c>
+      <c r="H8" s="5"/>
+    </row>
+    <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="2"/>
+    </row>
+    <row r="13" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    <row r="14" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="15" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
     <row r="17" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B17">
-        <v>0.05</v>
+      <c r="A17" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B18">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19">
         <v>0.2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B22">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23">
+        <f>G8/B22/B2</f>
+        <v>0.61189732142857145</v>
       </c>
     </row>
   </sheetData>

</xml_diff>